<commit_message>
Finished implementation of `dvg_ringbuffer_fir_filter`.
</commit_message>
<xml_diff>
--- a/FIR_filter_study/FIR_filter_convolution_scheme.xlsx
+++ b/FIR_filter_study/FIR_filter_convolution_scheme.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\_GitHub_repo\DvG_Arduino_lock-in_amp\FIR_filter_study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257ADAD4-0909-41BA-82F2-1868D0AE5DD6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DBCAECF-9E34-474C-B9AF-784B7FE45206}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="12405" windowWidth="25440" windowHeight="15540" xr2:uid="{954ABCBC-5CDF-4E6C-ABB2-AE0B044014B7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="28116" windowHeight="19416" xr2:uid="{954ABCBC-5CDF-4E6C-ABB2-AE0B044014B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$BE$56</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$BE$57</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="68">
   <si>
     <t>N_taps</t>
   </si>
@@ -141,12 +141,6 @@
     <t>T_valid_start</t>
   </si>
   <si>
-    <t>Dennis van Gils, 23-05-2021</t>
-  </si>
-  <si>
-    <t>i.e. Starting index within the input-signal ring buffer corresponding to the time stamps of the computed valid filter output</t>
-  </si>
-  <si>
     <t>BLOCK_SIZE</t>
   </si>
   <si>
@@ -156,9 +150,6 @@
     <t>N_blocks</t>
   </si>
   <si>
-    <t>Maximized N_taps given N_blocks</t>
-  </si>
-  <si>
     <t>= BLOCK_SIZE * N_blocks</t>
   </si>
   <si>
@@ -174,9 +165,6 @@
     <t>Perform convolve every incoming block, ring buffer is 3x BLOCK_SIZE</t>
   </si>
   <si>
-    <t>Perform convolve every incoming block, maximize N_taps given N_blocks</t>
-  </si>
-  <si>
     <t>ringbuffer idx:</t>
   </si>
   <si>
@@ -237,14 +225,29 @@
     <t>= (N_blocks - 1) * BLOCK_SIZE / Fs</t>
   </si>
   <si>
-    <t>i.e. When the filter starts outputting (not to be confused with the filter theoretical response time to an impulse)</t>
+    <t>Dennis van Gils, 24-05-2021</t>
+  </si>
+  <si>
+    <t>Maximized N_taps given BLOCK_SIZE and N_blocks</t>
+  </si>
+  <si>
+    <t>Perform convolve every incoming block, maximize N_taps given BLOCK_SIZE and N_blocks</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Note that the filter output lies in the past, namely at T_valid_start</t>
+  </si>
+  <si>
+    <t>i.e. Starting index within the input-signal ring buffer aligning to the time stamps of the computed valid filter output</t>
+  </si>
+  <si>
+    <t>i.e. Wallclock time when the filter starts outputting when being fed with incoming realtime data. Here, the term `settle` is not to be confused with the filter theoretical response time to an impulse.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -283,6 +286,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFC00000"/>
       <name val="Calibri"/>
@@ -632,12 +643,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -647,7 +659,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -967,9 +978,7 @@
   </sheetPr>
   <dimension ref="A1:BE79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:BE56"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -983,15 +992,15 @@
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I1" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G2"/>
     </row>
@@ -1002,59 +1011,59 @@
     </row>
     <row r="5" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="G5" s="63" t="s">
+      <c r="G5" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="64"/>
-      <c r="I5" s="64"/>
-      <c r="J5" s="64"/>
-      <c r="K5" s="64"/>
-      <c r="L5" s="64"/>
-      <c r="M5" s="64"/>
-      <c r="N5" s="64"/>
-      <c r="O5" s="64"/>
-      <c r="P5" s="65"/>
-      <c r="Q5" s="63" t="s">
+      <c r="H5" s="65"/>
+      <c r="I5" s="65"/>
+      <c r="J5" s="65"/>
+      <c r="K5" s="65"/>
+      <c r="L5" s="65"/>
+      <c r="M5" s="65"/>
+      <c r="N5" s="65"/>
+      <c r="O5" s="65"/>
+      <c r="P5" s="66"/>
+      <c r="Q5" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="R5" s="64"/>
-      <c r="S5" s="64"/>
-      <c r="T5" s="64"/>
-      <c r="U5" s="64"/>
-      <c r="V5" s="64"/>
-      <c r="W5" s="64"/>
-      <c r="X5" s="64"/>
-      <c r="Y5" s="64"/>
-      <c r="Z5" s="65"/>
-      <c r="AA5" s="63" t="s">
+      <c r="R5" s="65"/>
+      <c r="S5" s="65"/>
+      <c r="T5" s="65"/>
+      <c r="U5" s="65"/>
+      <c r="V5" s="65"/>
+      <c r="W5" s="65"/>
+      <c r="X5" s="65"/>
+      <c r="Y5" s="65"/>
+      <c r="Z5" s="66"/>
+      <c r="AA5" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="AB5" s="64"/>
-      <c r="AC5" s="64"/>
-      <c r="AD5" s="64"/>
-      <c r="AE5" s="64"/>
-      <c r="AF5" s="64"/>
-      <c r="AG5" s="64"/>
-      <c r="AH5" s="64"/>
-      <c r="AI5" s="64"/>
-      <c r="AJ5" s="65"/>
-      <c r="AK5" s="63" t="s">
+      <c r="AB5" s="65"/>
+      <c r="AC5" s="65"/>
+      <c r="AD5" s="65"/>
+      <c r="AE5" s="65"/>
+      <c r="AF5" s="65"/>
+      <c r="AG5" s="65"/>
+      <c r="AH5" s="65"/>
+      <c r="AI5" s="65"/>
+      <c r="AJ5" s="66"/>
+      <c r="AK5" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="AL5" s="64"/>
-      <c r="AM5" s="64"/>
-      <c r="AN5" s="64"/>
-      <c r="AO5" s="64"/>
-      <c r="AP5" s="64"/>
-      <c r="AQ5" s="64"/>
-      <c r="AR5" s="64"/>
-      <c r="AS5" s="64"/>
-      <c r="AT5" s="65"/>
+      <c r="AL5" s="65"/>
+      <c r="AM5" s="65"/>
+      <c r="AN5" s="65"/>
+      <c r="AO5" s="65"/>
+      <c r="AP5" s="65"/>
+      <c r="AQ5" s="65"/>
+      <c r="AR5" s="65"/>
+      <c r="AS5" s="65"/>
+      <c r="AT5" s="66"/>
       <c r="AU5" s="4"/>
     </row>
     <row r="6" spans="1:48" x14ac:dyDescent="0.3">
@@ -1170,7 +1179,7 @@
     </row>
     <row r="8" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B8" s="35">
         <v>10</v>
@@ -1186,91 +1195,91 @@
     </row>
     <row r="9" spans="1:48" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B9" s="35">
         <v>2</v>
       </c>
-      <c r="C9" s="60" t="s">
+      <c r="C9" s="59" t="s">
         <v>14</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G9" s="25"/>
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
       <c r="K9" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="L9" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="M9" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="N9" s="22"/>
       <c r="O9" s="22"/>
       <c r="P9" s="22"/>
       <c r="Q9" s="4"/>
       <c r="U9" s="10" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="V9" s="10" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="W9" s="10" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="X9" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="Y9" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="Z9" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="AA9" s="4"/>
       <c r="AE9" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="AF9" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="AG9" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="AH9" s="10" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="AI9" s="10" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="AJ9" s="10" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="AK9" s="4"/>
       <c r="AR9" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="AS9" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="AT9" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="AU9" s="4"/>
     </row>
     <row r="10" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B10" s="42">
         <f>B8*B9</f>
         <v>20</v>
       </c>
-      <c r="C10" s="60" t="s">
+      <c r="C10" s="59" t="s">
         <v>11</v>
       </c>
       <c r="G10" s="4"/>
@@ -1286,14 +1295,14 @@
       <c r="B11" s="52">
         <v>7</v>
       </c>
-      <c r="C11" s="60" t="s">
+      <c r="C11" s="59" t="s">
         <v>11</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G11" s="5">
         <v>0</v>
@@ -1427,7 +1436,7 @@
         <f>B8+B11-1</f>
         <v>16</v>
       </c>
-      <c r="C12" s="66" t="s">
+      <c r="C12" s="62" t="s">
         <v>11</v>
       </c>
       <c r="F12" s="29"/>
@@ -1474,13 +1483,13 @@
     </row>
     <row r="13" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="55" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B13" s="42">
         <f>B10-B12</f>
         <v>4</v>
       </c>
-      <c r="C13" s="60" t="s">
+      <c r="C13" s="59" t="s">
         <v>11</v>
       </c>
       <c r="G13" s="22"/>
@@ -1541,14 +1550,14 @@
         <f>B8</f>
         <v>10</v>
       </c>
-      <c r="C14" s="60" t="s">
+      <c r="C14" s="59" t="s">
         <v>11</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G14" s="5">
         <v>0</v>
@@ -1614,17 +1623,17 @@
     </row>
     <row r="15" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="55" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B15" s="42">
         <f>INT((B11-1)/2)</f>
         <v>3</v>
       </c>
-      <c r="C15" s="60" t="s">
+      <c r="C15" s="59" t="s">
         <v>11</v>
       </c>
       <c r="P15" s="7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="Q15" s="5">
         <v>0</v>
@@ -1689,17 +1698,17 @@
     </row>
     <row r="16" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="57" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B16" s="42">
         <f>B15+B13</f>
         <v>7</v>
       </c>
-      <c r="C16" s="60" t="s">
+      <c r="C16" s="59" t="s">
         <v>11</v>
       </c>
       <c r="Z16" s="7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="AA16" s="5">
         <v>0</v>
@@ -1769,76 +1778,76 @@
     </row>
     <row r="21" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="G21" s="63" t="s">
+        <v>43</v>
+      </c>
+      <c r="G21" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="H21" s="64"/>
-      <c r="I21" s="64"/>
-      <c r="J21" s="64"/>
-      <c r="K21" s="64"/>
-      <c r="L21" s="64"/>
-      <c r="M21" s="64"/>
-      <c r="N21" s="64"/>
-      <c r="O21" s="64"/>
-      <c r="P21" s="64"/>
-      <c r="Q21" s="63" t="s">
+      <c r="H21" s="65"/>
+      <c r="I21" s="65"/>
+      <c r="J21" s="65"/>
+      <c r="K21" s="65"/>
+      <c r="L21" s="65"/>
+      <c r="M21" s="65"/>
+      <c r="N21" s="65"/>
+      <c r="O21" s="65"/>
+      <c r="P21" s="65"/>
+      <c r="Q21" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="R21" s="64"/>
-      <c r="S21" s="64"/>
-      <c r="T21" s="64"/>
-      <c r="U21" s="64"/>
-      <c r="V21" s="64"/>
-      <c r="W21" s="64"/>
-      <c r="X21" s="64"/>
-      <c r="Y21" s="64"/>
-      <c r="Z21" s="64"/>
-      <c r="AA21" s="63" t="s">
+      <c r="R21" s="65"/>
+      <c r="S21" s="65"/>
+      <c r="T21" s="65"/>
+      <c r="U21" s="65"/>
+      <c r="V21" s="65"/>
+      <c r="W21" s="65"/>
+      <c r="X21" s="65"/>
+      <c r="Y21" s="65"/>
+      <c r="Z21" s="65"/>
+      <c r="AA21" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="AB21" s="64"/>
-      <c r="AC21" s="64"/>
-      <c r="AD21" s="64"/>
-      <c r="AE21" s="64"/>
-      <c r="AF21" s="64"/>
-      <c r="AG21" s="64"/>
-      <c r="AH21" s="64"/>
-      <c r="AI21" s="64"/>
-      <c r="AJ21" s="64"/>
-      <c r="AK21" s="63" t="s">
+      <c r="AB21" s="65"/>
+      <c r="AC21" s="65"/>
+      <c r="AD21" s="65"/>
+      <c r="AE21" s="65"/>
+      <c r="AF21" s="65"/>
+      <c r="AG21" s="65"/>
+      <c r="AH21" s="65"/>
+      <c r="AI21" s="65"/>
+      <c r="AJ21" s="65"/>
+      <c r="AK21" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="AL21" s="64"/>
-      <c r="AM21" s="64"/>
-      <c r="AN21" s="64"/>
-      <c r="AO21" s="64"/>
-      <c r="AP21" s="64"/>
-      <c r="AQ21" s="64"/>
-      <c r="AR21" s="64"/>
-      <c r="AS21" s="64"/>
-      <c r="AT21" s="64"/>
-      <c r="AU21" s="63" t="s">
+      <c r="AL21" s="65"/>
+      <c r="AM21" s="65"/>
+      <c r="AN21" s="65"/>
+      <c r="AO21" s="65"/>
+      <c r="AP21" s="65"/>
+      <c r="AQ21" s="65"/>
+      <c r="AR21" s="65"/>
+      <c r="AS21" s="65"/>
+      <c r="AT21" s="65"/>
+      <c r="AU21" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="AV21" s="64"/>
-      <c r="AW21" s="64"/>
-      <c r="AX21" s="64"/>
-      <c r="AY21" s="64"/>
-      <c r="AZ21" s="64"/>
-      <c r="BA21" s="64"/>
-      <c r="BB21" s="64"/>
-      <c r="BC21" s="64"/>
-      <c r="BD21" s="65"/>
+      <c r="AV21" s="65"/>
+      <c r="AW21" s="65"/>
+      <c r="AX21" s="65"/>
+      <c r="AY21" s="65"/>
+      <c r="AZ21" s="65"/>
+      <c r="BA21" s="65"/>
+      <c r="BB21" s="65"/>
+      <c r="BC21" s="65"/>
+      <c r="BD21" s="66"/>
       <c r="BE21" s="4"/>
     </row>
     <row r="22" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="24"/>
@@ -2010,12 +2019,12 @@
     </row>
     <row r="24" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B24" s="35">
         <v>10</v>
       </c>
-      <c r="C24" s="60" t="s">
+      <c r="C24" s="59" t="s">
         <v>11</v>
       </c>
       <c r="G24" s="25"/>
@@ -2072,178 +2081,178 @@
     </row>
     <row r="25" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B25" s="35">
         <v>3</v>
       </c>
-      <c r="C25" s="60" t="s">
+      <c r="C25" s="59" t="s">
         <v>14</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H25" s="27" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="I25" s="27" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J25" s="27" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="K25" s="27" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="L25" s="27" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="M25" s="27" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="N25" s="27" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="O25" s="27" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="P25" s="27" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="Q25" s="13" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="R25" s="28" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="S25" s="28" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="T25" s="28" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="U25" s="28" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="V25" s="28" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="W25" s="28" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="X25" s="28" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="Y25" s="28" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="Z25" s="28" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="AA25" s="11" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="AB25" s="27" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="AC25" s="27" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="AD25" s="27" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="AE25" s="27" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="AF25" s="27" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="AG25" s="27" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="AH25" s="27" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="AI25" s="27" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="AJ25" s="27" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="AK25" s="13" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="AL25" s="28" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="AM25" s="28" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="AN25" s="28" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="AO25" s="28" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="AP25" s="28" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="AQ25" s="28" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="AR25" s="28" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="AS25" s="28" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="AT25" s="28" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="AU25" s="11" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="AV25" s="27" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="AW25" s="27" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="AX25" s="27" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="AY25" s="27" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="AZ25" s="27" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="BA25" s="27" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="BB25" s="27" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="BC25" s="27" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="BD25" s="27" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="BE25" s="25"/>
     </row>
     <row r="26" spans="1:57" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B26" s="43">
         <f>B24*B25</f>
         <v>30</v>
       </c>
-      <c r="C26" s="60" t="s">
+      <c r="C26" s="59" t="s">
         <v>11</v>
       </c>
       <c r="G26" s="25"/>
@@ -2267,34 +2276,34 @@
       <c r="Y26" s="14"/>
       <c r="Z26" s="14"/>
       <c r="AA26" s="11" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="AB26" s="27" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="AC26" s="27" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="AD26" s="27" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="AE26" s="27" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="AF26" s="27" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="AG26" s="27" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="AH26" s="27" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="AI26" s="27" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="AJ26" s="27" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="AK26" s="4"/>
       <c r="AL26" s="24"/>
@@ -2325,14 +2334,14 @@
       <c r="B27" s="52">
         <v>21</v>
       </c>
-      <c r="C27" s="60" t="s">
+      <c r="C27" s="59" t="s">
         <v>11</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G27" s="5">
         <v>0</v>
@@ -2496,7 +2505,7 @@
         <f>B24+B27-1</f>
         <v>30</v>
       </c>
-      <c r="C28" s="66" t="s">
+      <c r="C28" s="62" t="s">
         <v>11</v>
       </c>
       <c r="G28" s="22"/>
@@ -2543,13 +2552,13 @@
     </row>
     <row r="29" spans="1:57" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="55" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B29" s="43">
         <f>B26-B28</f>
         <v>0</v>
       </c>
-      <c r="C29" s="60" t="s">
+      <c r="C29" s="59" t="s">
         <v>11</v>
       </c>
       <c r="G29" s="22"/>
@@ -2602,14 +2611,14 @@
         <f>B24</f>
         <v>10</v>
       </c>
-      <c r="C30" s="60" t="s">
+      <c r="C30" s="59" t="s">
         <v>11</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G30" s="30">
         <v>0</v>
@@ -2715,13 +2724,13 @@
     </row>
     <row r="31" spans="1:57" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="55" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B31" s="43">
         <f>INT((B27-1)/2)</f>
         <v>10</v>
       </c>
-      <c r="C31" s="60" t="s">
+      <c r="C31" s="59" t="s">
         <v>11</v>
       </c>
       <c r="G31" s="22"/>
@@ -2734,7 +2743,7 @@
       <c r="N31" s="22"/>
       <c r="O31" s="22"/>
       <c r="P31" s="26" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="Q31" s="34">
         <v>0</v>
@@ -2830,13 +2839,13 @@
     </row>
     <row r="32" spans="1:57" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="57" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B32" s="43">
         <f>B31+B29</f>
         <v>10</v>
       </c>
-      <c r="C32" s="60" t="s">
+      <c r="C32" s="59" t="s">
         <v>11</v>
       </c>
       <c r="G32" s="22"/>
@@ -2859,7 +2868,7 @@
       <c r="X32" s="22"/>
       <c r="Y32" s="22"/>
       <c r="Z32" s="26" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="AA32" s="30">
         <v>0</v>
@@ -2959,7 +2968,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="37" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="B36" s="37"/>
       <c r="C36" s="37"/>
@@ -2982,7 +2991,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="58" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B39" s="35">
         <v>2000</v>
@@ -2993,7 +3002,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="58" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B40" s="35">
         <v>21</v>
@@ -3004,7 +3013,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B42" s="43">
         <f>B39*B40</f>
@@ -3014,7 +3023,7 @@
         <v>11</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
@@ -3029,7 +3038,7 @@
         <v>11</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
@@ -3093,12 +3102,12 @@
         <v>11</v>
       </c>
       <c r="D50" s="50" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="55" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B51" s="43">
         <f>B42-B50</f>
@@ -3108,7 +3117,7 @@
         <v>11</v>
       </c>
       <c r="D51" s="50" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
@@ -3123,12 +3132,12 @@
         <v>11</v>
       </c>
       <c r="D52" s="49" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="55" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B53" s="43">
         <f>INT((B43-1)/2)</f>
@@ -3143,7 +3152,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="53" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B54" s="43">
         <f>B51+B53</f>
@@ -3153,29 +3162,29 @@
         <v>11</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" s="60" t="s">
+      <c r="A55" s="59" t="s">
         <v>33</v>
       </c>
       <c r="B55" s="44">
         <f>B54/B38</f>
         <v>1</v>
       </c>
-      <c r="C55" s="61" t="s">
+      <c r="C55" s="60" t="s">
         <v>16</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G55" s="59" t="s">
-        <v>35</v>
+        <v>39</v>
+      </c>
+      <c r="G55" s="63" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" s="62" t="s">
+      <c r="A56" s="61" t="s">
         <v>32</v>
       </c>
       <c r="B56" s="44">
@@ -3186,10 +3195,15 @@
         <v>16</v>
       </c>
       <c r="D56" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G56" s="63" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G57" s="63" t="s">
         <v>65</v>
-      </c>
-      <c r="G56" s="59" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
@@ -3199,7 +3213,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
@@ -3215,7 +3229,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B62" s="35">
         <v>500</v>
@@ -3243,7 +3257,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B65" s="43">
         <f>1+(B63-1)/B62</f>
@@ -3255,7 +3269,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B66" s="43">
         <f>_xlfn.CEILING.MATH(B65)</f>
@@ -3267,7 +3281,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B67" s="43">
         <f>B62*B66</f>
@@ -3340,7 +3354,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="55" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B75" s="43">
         <f>B67-B74</f>
@@ -3362,12 +3376,12 @@
         <v>11</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="55" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B77" s="43">
         <f>INT((B63-1)/2)</f>
@@ -3379,7 +3393,7 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="53" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B78" s="43">
         <f>B77+B75</f>

</xml_diff>